<commit_message>
added 3 rice bsseq
</commit_message>
<xml_diff>
--- a/rice.xlsx
+++ b/rice.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/25894C72-A658-4463-B76F-C107C5CA2B7A/login.msi.umn.edu/panfs/roc/groups/15/springer/zhoux379/projects/barn/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orion/Library/Containers/com.panic.transmit.mas/Data/Library/Caches/Transmit/0C5E832B-3EE0-4F1E-A72E-CB6D0C8FC111/login.msi.umn.edu/panfs/roc/groups/15/springer/zhoux379/projects/barn/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0B7ACC-1E57-7943-970D-45566FBA19C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034802DE-1CEF-6146-BE4C-64D9C7B798B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12240" yWindow="4720" windowWidth="20540" windowHeight="16280" xr2:uid="{5C1DF351-30C1-7A41-98E1-E0C48EB7ED9F}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="rice" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Z_03A8949B_C78E_4E7F_9412_8C36B64964FE_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$11</definedName>
-    <definedName name="Z_0C26BD42_2CBD_4138_9861_6D4EEF11FB87_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$11</definedName>
-    <definedName name="Z_32787278_35C0_4446_BB99_F1281F67D683_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$11</definedName>
-    <definedName name="Z_610B8B3C_8CF9_4F7D_B2D6_4264B7FE77F8_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$11</definedName>
-    <definedName name="Z_8E992A79_4279_4BA5_8ACA_2AFCD1FF395F_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$11</definedName>
-    <definedName name="Z_A1ED0A0E_827F_4174_B807_FE6BA2FB73B4_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$11</definedName>
-    <definedName name="Z_C21AEDBF_7EB1_42BD_A502_AF69742EFC77_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$11</definedName>
-    <definedName name="Z_DBE29AA5_4612_41A5_AA32_A789BF2A0694_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$11</definedName>
+    <definedName name="Z_03A8949B_C78E_4E7F_9412_8C36B64964FE_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$12</definedName>
+    <definedName name="Z_0C26BD42_2CBD_4138_9861_6D4EEF11FB87_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$12</definedName>
+    <definedName name="Z_32787278_35C0_4446_BB99_F1281F67D683_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$12</definedName>
+    <definedName name="Z_610B8B3C_8CF9_4F7D_B2D6_4264B7FE77F8_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$12</definedName>
+    <definedName name="Z_8E992A79_4279_4BA5_8ACA_2AFCD1FF395F_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$12</definedName>
+    <definedName name="Z_A1ED0A0E_827F_4174_B807_FE6BA2FB73B4_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$12</definedName>
+    <definedName name="Z_C21AEDBF_7EB1_42BD_A502_AF69742EFC77_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$12</definedName>
+    <definedName name="Z_DBE29AA5_4612_41A5_AA32_A789BF2A0694_.wvu.FilterData" localSheetId="0" hidden="1">rice!$A$1:$R$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="66">
   <si>
     <t>rnaseq</t>
   </si>
@@ -211,13 +211,37 @@
     <t>bs16b</t>
   </si>
   <si>
-    <t>PRJCA000239</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
-    <t>seed germination</t>
+    <t>Tan</t>
+  </si>
+  <si>
+    <t>PRJNA321532</t>
+  </si>
+  <si>
+    <t>rice ddm1 and drm2</t>
+  </si>
+  <si>
+    <t>bs12b</t>
+  </si>
+  <si>
+    <t>SRP002084</t>
+  </si>
+  <si>
+    <t>transriptome and methylome</t>
+  </si>
+  <si>
+    <t>4 rice</t>
+  </si>
+  <si>
+    <t>mo20b</t>
+  </si>
+  <si>
+    <t>Zhao</t>
+  </si>
+  <si>
+    <t>PRJNA597475</t>
+  </si>
+  <si>
+    <t>20 rice epigenome</t>
   </si>
 </sst>
 </file>
@@ -677,11 +701,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -803,32 +827,34 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3">
+        <v>4</v>
+      </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
@@ -841,36 +867,32 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E4" s="3">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="3">
-        <v>3</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="3">
-        <v>3</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -883,14 +905,14 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3">
         <v>2015</v>
@@ -899,16 +921,20 @@
         <v>1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
       <c r="J5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <v>3</v>
+      </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
@@ -921,34 +947,32 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E6" s="3">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="K6" s="3">
-        <v>1</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -961,14 +985,14 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="E7" s="3">
         <v>2016</v>
@@ -977,17 +1001,17 @@
         <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="K7" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -1001,50 +1025,48 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>54</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4">
-        <v>2020</v>
+      <c r="D8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2016</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3">
-        <v>12</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="4">
-        <v>12</v>
+      <c r="K8" s="3">
+        <v>3</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="3"/>
       <c r="O8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" s="5" t="str">
-        <f>HYPERLINK(CONCATENATE("", "https://orionzhou.github.io/public/multiqc/", A8, ".html"), A8)</f>
-        <v>mo20a</v>
-      </c>
-      <c r="Q8" s="5" t="str">
-        <f>HYPERLINK(CONCATENATE("", "https://github.com/orionzhou/",O8,"/tree/master/data/11_qc/", A8, ""), A8)</f>
-        <v>mo20a</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1055,38 +1077,36 @@
         <v>26</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="H9" s="3"/>
       <c r="I9" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="N9" s="1"/>
       <c r="O9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P9" s="5" t="str">
         <f>HYPERLINK(CONCATENATE("", "https://orionzhou.github.io/public/multiqc/", A9, ".html"), A9)</f>
-        <v>mo20a2</v>
+        <v>mo20a</v>
       </c>
       <c r="Q9" s="5" t="str">
         <f>HYPERLINK(CONCATENATE("", "https://github.com/orionzhou/",O9,"/tree/master/data/11_qc/", A9, ""), A9)</f>
-        <v>mo20a2</v>
+        <v>mo20a</v>
       </c>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1101,34 +1121,34 @@
         <v>27</v>
       </c>
       <c r="I10" s="3">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="4">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="1" t="s">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="P10" s="5" t="str">
         <f>HYPERLINK(CONCATENATE("", "https://orionzhou.github.io/public/multiqc/", A10, ".html"), A10)</f>
-        <v>mo20a3</v>
+        <v>mo20a2</v>
       </c>
       <c r="Q10" s="5" t="str">
         <f>HYPERLINK(CONCATENATE("", "https://github.com/orionzhou/",O10,"/tree/master/data/11_qc/", A10, ""), A10)</f>
-        <v>mo20a3</v>
+        <v>mo20a2</v>
       </c>
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1143,70 +1163,157 @@
         <v>27</v>
       </c>
       <c r="I11" s="3">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="4">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="P11" s="5" t="str">
         <f>HYPERLINK(CONCATENATE("", "https://orionzhou.github.io/public/multiqc/", A11, ".html"), A11)</f>
-        <v>mo20a4</v>
-      </c>
-      <c r="Q11" s="2" t="str">
+        <v>mo20a3</v>
+      </c>
+      <c r="Q11" s="5" t="str">
         <f>HYPERLINK(CONCATENATE("", "https://github.com/orionzhou/",O11,"/tree/master/data/11_qc/", A11, ""), A11)</f>
-        <v>mo20a4</v>
+        <v>mo20a3</v>
       </c>
       <c r="R11" s="1"/>
     </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4">
+        <v>2020</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="3">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4">
+        <v>8</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("", "https://orionzhou.github.io/public/multiqc/", A12, ".html"), A12)</f>
+        <v>mo20a4</v>
+      </c>
+      <c r="Q12" s="2" t="str">
+        <f>HYPERLINK(CONCATENATE("", "https://github.com/orionzhou/",O12,"/tree/master/data/11_qc/", A12, ""), A12)</f>
+        <v>mo20a4</v>
+      </c>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="3">
+        <v>2020</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="3">
+        <v>20</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="3">
+        <v>20</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1" t="str">
+        <f>HYPERLINK(CONCATENATE("", "https://github.com/orionzhou/",O13,"/tree/master/data/11_qc/", A13, ""), A13)</f>
+        <v>mo20b</v>
+      </c>
+      <c r="R13" s="1"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:N11 R1:R11">
+  <conditionalFormatting sqref="L1:N13 R1:R13">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"T"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8:O11 B1:B11">
+  <conditionalFormatting sqref="O9:O13 B1:B13">
     <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"rnaseq"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8:O11 B1:B11">
+  <conditionalFormatting sqref="O9:O13 B1:B13">
     <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"chipseq"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8:O11 B1:B11">
+  <conditionalFormatting sqref="O9:O13 B1:B13">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"dnaseq"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8:O11 B1:B11">
+  <conditionalFormatting sqref="O9:O13 B1:B13">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"dapseq"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8:O11 B1:B11">
+  <conditionalFormatting sqref="O9:O13 B1:B13">
     <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"methylseq"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8:O11 B1:B11">
+  <conditionalFormatting sqref="O9:O13 B1:B13">
     <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"atacseq"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O8:O11 B1:B11">
+  <conditionalFormatting sqref="O9:O13 B1:B13">
     <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>"smrnaseq"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R1:R11">
+  <conditionalFormatting sqref="R1:R13">
     <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>"C"</formula>
     </cfRule>

</xml_diff>